<commit_message>
modified:   LTE_TX_SPURIOUS_attach_Tx.py 	modified:   config.json
</commit_message>
<xml_diff>
--- a/Band2MaxPowerInput.xlsx
+++ b/Band2MaxPowerInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\LTE_TX_SPUR_EMISSIONS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\DVT-Wireless-HCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A439CAD1-F327-46F0-85A0-7EF3AF97C6B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0980614-9BC2-4701-9FE2-E2A9DDBDD5A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>
   <sheets>
     <sheet name="Band2" sheetId="1" r:id="rId1"/>
@@ -2155,7 +2155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8596D56-7C71-4D72-A666-9CAEA981CBE7}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -4312,7 +4312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDABD784-AD31-46F2-99DC-A4DD1B41AE1B}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>